<commit_message>
Details and Type intent functionalities added.
</commit_message>
<xml_diff>
--- a/data/football_records_table.xlsx
+++ b/data/football_records_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d54d85b42225de07/Work/SEBIS/Teaching/CAI/Data/sports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cemuyuk/Desktop/Conversational AI/FootballRecordBot/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_BB3824CE2D0D6C56B1B434C062EF6133B2D3B5E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A79B0B4D-C3A9-4D01-A17F-68D6868FF8A6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8E80EF-0331-2E49-8A6F-C37406F0E4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sports_data" sheetId="1" r:id="rId1"/>
@@ -1416,48 +1416,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1753,15 +1753,18 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="58.5" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1801,7 +1804,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1821,7 +1824,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1841,7 +1844,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1881,7 +1884,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1941,7 +1944,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1961,7 +1964,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1981,7 +1984,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2021,7 +2024,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -2041,7 +2044,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -2161,7 +2164,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -2201,7 +2204,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -2241,7 +2244,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -2281,7 +2284,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2301,7 +2304,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -2341,7 +2344,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>122</v>
       </c>
@@ -2401,7 +2404,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -2421,7 +2424,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>133</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>136</v>
       </c>
@@ -2481,7 +2484,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>138</v>
       </c>
@@ -2501,7 +2504,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>139</v>
       </c>
@@ -2521,7 +2524,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -2541,7 +2544,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>148</v>
       </c>
@@ -2561,7 +2564,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -2581,7 +2584,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>157</v>
       </c>
@@ -2601,7 +2604,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>159</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>164</v>
       </c>
@@ -2641,7 +2644,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>168</v>
       </c>
@@ -2661,7 +2664,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>171</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>175</v>
       </c>
@@ -2701,7 +2704,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>180</v>
       </c>
@@ -2721,7 +2724,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>184</v>
       </c>
@@ -2741,7 +2744,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>189</v>
       </c>
@@ -2761,7 +2764,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>192</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>194</v>
       </c>
@@ -2801,7 +2804,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>198</v>
       </c>
@@ -2821,7 +2824,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>202</v>
       </c>
@@ -2841,7 +2844,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>207</v>
       </c>
@@ -2861,7 +2864,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>211</v>
       </c>
@@ -2881,7 +2884,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>216</v>
       </c>
@@ -2901,7 +2904,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>220</v>
       </c>
@@ -2921,7 +2924,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>224</v>
       </c>
@@ -2941,7 +2944,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>229</v>
       </c>
@@ -2961,7 +2964,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>233</v>
       </c>
@@ -2981,7 +2984,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>237</v>
       </c>
@@ -3001,7 +3004,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>242</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>246</v>
       </c>
@@ -3041,7 +3044,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>248</v>
       </c>
@@ -3061,7 +3064,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>252</v>
       </c>
@@ -3081,7 +3084,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>256</v>
       </c>
@@ -3101,7 +3104,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>261</v>
       </c>
@@ -3121,7 +3124,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>264</v>
       </c>
@@ -3141,7 +3144,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>268</v>
       </c>
@@ -3161,7 +3164,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>271</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>274</v>
       </c>
@@ -3201,7 +3204,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>279</v>
       </c>
@@ -3221,7 +3224,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>282</v>
       </c>
@@ -3238,7 +3241,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>285</v>
       </c>
@@ -3258,7 +3261,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>289</v>
       </c>
@@ -3278,7 +3281,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>293</v>
       </c>
@@ -3295,7 +3298,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>296</v>
       </c>

</xml_diff>